<commit_message>
[R/loadWorkbook] fix reading external links
</commit_message>
<xml_diff>
--- a/inst/extdata/mtcars_chart.xlsx
+++ b/inst/extdata/mtcars_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janmarvingarbuszus/Source/openxlsx2/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D262EF6-4BE1-9D48-BC51-9BD4995F49EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C30F8E4-C2FB-EA46-B26A-18680C4AD218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="1260" windowWidth="30240" windowHeight="17580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,8 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1431,6 +1433,72 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="IrisSample"/>
+      <sheetName val="testing"/>
+      <sheetName val="mtcars"/>
+      <sheetName val="mtCars Pivot"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>6.4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet 3"/>
+      <sheetName val="Sheet 4"/>
+      <sheetName val="Sheet 5"/>
+      <sheetName val="Sheet 6"/>
+      <sheetName val="1"/>
+      <sheetName val="11"/>
+      <sheetName val="111"/>
+      <sheetName val="1111"/>
+      <sheetName val="11111"/>
+      <sheetName val="111111"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6">
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2881,10 +2949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B65C424-8BC7-F74E-905D-7974903EE0B9}">
-  <dimension ref="B5:C5"/>
+  <dimension ref="B5:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2898,6 +2966,18 @@
         <v>1000000</v>
       </c>
     </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>[2]IrisSample!$A$2</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f>'[3]1'!$A$2</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[R/loadWorkbook] Fix reading external links (#125)
</commit_message>
<xml_diff>
--- a/inst/extdata/mtcars_chart.xlsx
+++ b/inst/extdata/mtcars_chart.xlsx
@@ -8,15 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janmarvingarbuszus/Source/openxlsx2/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CA8D5B3-3915-434C-9A51-605DBBF944DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C30F8E4-C2FB-EA46-B26A-18680C4AD218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="test" sheetId="1" r:id="rId2"/>
+    <sheet name="Ext" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -89,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,7 +1371,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{16FE037F-31F5-604F-9223-1020852C879A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1390,6 +1409,94 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="SUM"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="B6">
+            <v>44197</v>
+          </cell>
+          <cell r="C6">
+            <v>1000000</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="IrisSample"/>
+      <sheetName val="testing"/>
+      <sheetName val="mtcars"/>
+      <sheetName val="mtCars Pivot"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>6.4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet 3"/>
+      <sheetName val="Sheet 4"/>
+      <sheetName val="Sheet 5"/>
+      <sheetName val="Sheet 6"/>
+      <sheetName val="1"/>
+      <sheetName val="11"/>
+      <sheetName val="111"/>
+      <sheetName val="1111"/>
+      <sheetName val="11111"/>
+      <sheetName val="111111"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6">
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2838,4 +2945,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B65C424-8BC7-F74E-905D-7974903EE0B9}">
+  <dimension ref="B5:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>44197</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(B5,[1]SUM!$B$6:$C$6,2,FALSE)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>[2]IrisSample!$A$2</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f>'[3]1'!$A$2</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[R/extdata] add embeddings example
</commit_message>
<xml_diff>
--- a/inst/extdata/mtcars_chart.xlsx
+++ b/inst/extdata/mtcars_chart.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janmarvingarbuszus/Source/openxlsx2/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C30F8E4-C2FB-EA46-B26A-18680C4AD218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746EFC62-5FA2-5D4F-A0D4-31524C281AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="test" sheetId="1" r:id="rId2"/>
     <sheet name="Ext" sheetId="3" r:id="rId3"/>
+    <sheet name="Emb" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1411,6 +1412,79 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>50800</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>444500</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4097" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4097"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6C63BBB-AF91-B042-B21C-43DBFA115303}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects>
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="808080"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -2951,7 +3025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B65C424-8BC7-F74E-905D-7974903EE0B9}">
   <dimension ref="B5:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2981,4 +3055,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A916E692-8726-2D47-995F-1C1047AB69E1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Word.Document.12" dvAspect="DVASPECT_ICON" shapeId="4097" r:id="rId3">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>50800</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>444500</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Word.Document.12" dvAspect="DVASPECT_ICON" shapeId="4097" r:id="rId3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixes for clone_worksheet with tables, charts and drawings
</commit_message>
<xml_diff>
--- a/inst/extdata/mtcars_chart.xlsx
+++ b/inst/extdata/mtcars_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janmarvingarbuszus/Source/openxlsx2/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746EFC62-5FA2-5D4F-A0D4-31524C281AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B946098-855B-F549-A696-D395624A2A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -825,7 +825,1143 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>22.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>test!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cyl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>disp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>drat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>wt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vs</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>am</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>gear</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>test!$A$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>24.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-5C3E-6447-BF8C-372DDCD011D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2020301296"/>
+        <c:axId val="2020397296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2020301296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2020397296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2020397296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2020301296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1015,6 +2151,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1414,6 +3066,47 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D490715-BEB7-5319-ED6F-A9C49E8672B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -1437,7 +3130,7 @@
                   <a14:compatExt spid="_x0000_s4097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6C63BBB-AF91-B042-B21C-43DBFA115303}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1458,23 +3151,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1854,8 +3534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3018,6 +4698,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3061,7 +4742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A916E692-8726-2D47-995F-1C1047AB69E1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>